<commit_message>
Madras to host District meet 1
</commit_message>
<xml_diff>
--- a/docs/2020-2021_season/_study_schedule.xlsx
+++ b/docs/2020-2021_season/_study_schedule.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gryphon\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\pnwquizzing\docs\2020-2021_season\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33435" windowHeight="17730" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32160" windowHeight="17730" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Old" sheetId="1" r:id="rId1"/>
+    <sheet name="Current" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Old!$A$1:$E$55</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="82">
   <si>
     <t>Chapter</t>
   </si>
@@ -279,6 +279,12 @@
   </si>
   <si>
     <t>Overall Totals</t>
+  </si>
+  <si>
+    <t>October 23-24, 2020</t>
+  </si>
+  <si>
+    <t>District Champs</t>
   </si>
 </sst>
 </file>
@@ -989,9 +995,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1014,6 +1017,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1297,8 +1303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1313,22 +1319,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="81" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
     </row>
     <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H3" s="48"/>
@@ -1969,12 +1975,12 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="70" t="s">
+      <c r="A55" s="69" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="70" t="s">
+      <c r="B56" s="69" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1984,7 +1990,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="71" t="s">
+      <c r="B58" s="70" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2010,7 +2016,7 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2021,41 +2027,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="81" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
     </row>
     <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="78" t="s">
+      <c r="C4" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="78" t="s">
+      <c r="D4" s="77" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="80" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -2069,7 +2075,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="80" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -2083,7 +2089,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="80" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -2097,7 +2103,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="80" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -2111,29 +2117,29 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="79" t="s">
+      <c r="A9" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="79" t="s">
+      <c r="B9" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="78">
+      <c r="C9" s="77">
         <f>SUM(C5:C8)</f>
         <v>73</v>
       </c>
-      <c r="D9" s="78">
+      <c r="D9" s="77">
         <f>SUM(D5:D8)</f>
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="72"/>
-      <c r="B10" s="74"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="80" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -2147,7 +2153,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="80" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -2161,7 +2167,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="80" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -2175,43 +2181,43 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="80" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="7">
+        <v>34</v>
+      </c>
+      <c r="D14" s="7">
         <v>6</v>
       </c>
-      <c r="B14" s="79" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="78">
-        <f>SUM(C11:C13,C9)</f>
-        <v>184</v>
-      </c>
-      <c r="D14" s="78">
-        <f>SUM(D11:D13,D9)</f>
-        <v>107</v>
-      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="72"/>
-      <c r="B15" s="74"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
+      <c r="A15" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="78" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="77">
+        <f>SUM(C11:C14)</f>
+        <v>145</v>
+      </c>
+      <c r="D15" s="77">
+        <f>SUM(D11:D14)</f>
+        <v>86</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="81" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="7">
-        <v>34</v>
-      </c>
-      <c r="D16" s="7">
-        <v>6</v>
-      </c>
+      <c r="A16" s="71"/>
+      <c r="B16" s="73"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="74"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="81" t="s">
+      <c r="A17" s="80" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -2225,7 +2231,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="81" t="s">
+      <c r="A18" s="80" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -2239,7 +2245,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="81" t="s">
+      <c r="A19" s="80" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="6" t="s">
@@ -2253,7 +2259,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="81" t="s">
+      <c r="A20" s="80" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="6" t="s">
@@ -2267,32 +2273,32 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="79" t="s">
+      <c r="A21" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="79" t="s">
+      <c r="B21" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="78">
-        <f>SUM(C16:C20)</f>
-        <v>194</v>
-      </c>
-      <c r="D21" s="78">
-        <f>SUM(D16:D20)</f>
-        <v>65</v>
+      <c r="C21" s="77">
+        <f>SUM(C17:C20)</f>
+        <v>160</v>
+      </c>
+      <c r="D21" s="77">
+        <f>SUM(D17:D20)</f>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="72"/>
-      <c r="B22" s="74"/>
-      <c r="C22" s="75"/>
-      <c r="D22" s="75"/>
+      <c r="A22" s="71"/>
+      <c r="B22" s="73"/>
+      <c r="C22" s="74"/>
+      <c r="D22" s="74"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="81" t="s">
+      <c r="A23" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="80">
+      <c r="B23" s="79">
         <v>33</v>
       </c>
       <c r="C23" s="7">
@@ -2303,7 +2309,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="81" t="s">
+      <c r="A24" s="80" t="s">
         <v>37</v>
       </c>
       <c r="B24" s="6" t="s">
@@ -2317,7 +2323,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="81" t="s">
+      <c r="A25" s="80" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="6" t="s">
@@ -2331,7 +2337,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="81" t="s">
+      <c r="A26" s="80" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="6" t="s">
@@ -2345,7 +2351,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="81" t="s">
+      <c r="A27" s="80" t="s">
         <v>40</v>
       </c>
       <c r="B27" s="6" t="s">
@@ -2359,29 +2365,29 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="79" t="s">
+      <c r="A28" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="79" t="s">
+      <c r="B28" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="78">
+      <c r="C28" s="77">
         <f>SUM(C23:C27)</f>
         <v>165</v>
       </c>
-      <c r="D28" s="78">
+      <c r="D28" s="77">
         <f>SUM(D23:D27)</f>
         <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="72"/>
-      <c r="B29" s="74"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="75"/>
+      <c r="A29" s="71"/>
+      <c r="B29" s="73"/>
+      <c r="C29" s="74"/>
+      <c r="D29" s="74"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="81" t="s">
+      <c r="A30" s="80" t="s">
         <v>41</v>
       </c>
       <c r="B30" s="6" t="s">
@@ -2395,7 +2401,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="81" t="s">
+      <c r="A31" s="80" t="s">
         <v>42</v>
       </c>
       <c r="B31" s="6" t="s">
@@ -2409,7 +2415,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="81" t="s">
+      <c r="A32" s="80" t="s">
         <v>43</v>
       </c>
       <c r="B32" s="6" t="s">
@@ -2423,7 +2429,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="81" t="s">
+      <c r="A33" s="80" t="s">
         <v>44</v>
       </c>
       <c r="B33" s="6" t="s">
@@ -2437,29 +2443,29 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="79" t="s">
+      <c r="A34" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="79" t="s">
+      <c r="B34" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="78">
+      <c r="C34" s="77">
         <f>SUM(C30:C33)</f>
         <v>156</v>
       </c>
-      <c r="D34" s="78">
+      <c r="D34" s="77">
         <f>SUM(D30:D33)</f>
         <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="72"/>
-      <c r="B35" s="74"/>
-      <c r="C35" s="75"/>
-      <c r="D35" s="75"/>
+      <c r="A35" s="71"/>
+      <c r="B35" s="73"/>
+      <c r="C35" s="74"/>
+      <c r="D35" s="74"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="81" t="s">
+      <c r="A36" s="80" t="s">
         <v>45</v>
       </c>
       <c r="B36" s="6" t="s">
@@ -2473,7 +2479,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="81" t="s">
+      <c r="A37" s="80" t="s">
         <v>46</v>
       </c>
       <c r="B37" s="6" t="s">
@@ -2487,7 +2493,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="81" t="s">
+      <c r="A38" s="80" t="s">
         <v>47</v>
       </c>
       <c r="B38" s="6" t="s">
@@ -2501,67 +2507,67 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="79" t="s">
+      <c r="A39" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="79" t="s">
+      <c r="B39" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="78">
+      <c r="C39" s="77">
         <f>SUM(C36:C38)</f>
         <v>161</v>
       </c>
-      <c r="D39" s="78">
+      <c r="D39" s="77">
         <f>SUM(D36:D38)</f>
         <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C40" s="73"/>
-      <c r="D40" s="73"/>
+      <c r="C40" s="72"/>
+      <c r="D40" s="72"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="76" t="s">
+      <c r="B41" s="75" t="s">
         <v>79</v>
       </c>
-      <c r="C41" s="78">
-        <f>SUM(C14,C21,C28,C34,C39)</f>
+      <c r="C41" s="77">
+        <f>SUM(C9,C15,C21,C28,C34,C39)</f>
         <v>860</v>
       </c>
-      <c r="D41" s="78">
-        <f>SUM(D14,D21,D28,D34,D39)</f>
+      <c r="D41" s="77">
+        <f>SUM(D9,D15,D21,D28,D34,D39)</f>
         <v>311</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="79" t="s">
+      <c r="A43" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="B43" s="77" t="s">
+      <c r="B43" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="75"/>
-      <c r="D43" s="75"/>
+      <c r="C43" s="74"/>
+      <c r="D43" s="74"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="79" t="s">
-        <v>12</v>
-      </c>
-      <c r="B44" s="77" t="s">
+      <c r="A44" s="78" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="C44" s="75"/>
-      <c r="D44" s="75"/>
+      <c r="C44" s="74"/>
+      <c r="D44" s="74"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="79" t="s">
+      <c r="A45" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="77" t="s">
+      <c r="B45" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="75"/>
-      <c r="D45" s="75"/>
+      <c r="C45" s="74"/>
+      <c r="D45" s="74"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
@@ -2583,14 +2589,14 @@
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="70" t="s">
+      <c r="A49" s="69" t="s">
         <v>77</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="70" t="s">
+      <c r="B50" s="69" t="s">
         <v>76</v>
       </c>
       <c r="C50" s="3"/>
@@ -2604,7 +2610,7 @@
       <c r="D51" s="3"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="71" t="s">
+      <c r="B52" s="70" t="s">
         <v>75</v>
       </c>
       <c r="C52" s="3"/>
@@ -2619,6 +2625,6 @@
     <hyperlink ref="B52" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="87" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup scale="86" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove 15:21 from the KVL
</commit_message>
<xml_diff>
--- a/docs/2020-2021_season/_study_schedule.xlsx
+++ b/docs/2020-2021_season/_study_schedule.xlsx
@@ -199,9 +199,6 @@
     <t>6, 8, 11, 12, 18-21, 25, 26, 30, 31, 32, 34-37, 40, 49, 50</t>
   </si>
   <si>
-    <t>8, 9, 11, 13, 14, 18-21, 32</t>
-  </si>
-  <si>
     <t>4, 6, 16-19, 21, 23, 24, 26, 27</t>
   </si>
   <si>
@@ -266,6 +263,9 @@
   </si>
   <si>
     <t>December 4-5, 2020</t>
+  </si>
+  <si>
+    <t>8, 9, 11, 13, 14, 18-20, 32</t>
   </si>
 </sst>
 </file>
@@ -676,7 +676,7 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,7 +688,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -717,7 +717,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -859,7 +859,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" s="15">
         <f>SUM(C11:C14)</f>
@@ -937,7 +937,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C21" s="15">
         <f>SUM(C17:C20)</f>
@@ -973,7 +973,7 @@
         <v>31</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="C24" s="4">
         <v>39</v>
@@ -987,7 +987,7 @@
         <v>32</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="4">
         <v>28</v>
@@ -1001,7 +1001,7 @@
         <v>33</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" s="4">
         <v>27</v>
@@ -1015,7 +1015,7 @@
         <v>34</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" s="4">
         <v>35</v>
@@ -1051,7 +1051,7 @@
         <v>35</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C30" s="4">
         <v>30</v>
@@ -1065,7 +1065,7 @@
         <v>36</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C31" s="4">
         <v>34</v>
@@ -1079,7 +1079,7 @@
         <v>37</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C32" s="4">
         <v>46</v>
@@ -1093,7 +1093,7 @@
         <v>38</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C33" s="4">
         <v>46</v>
@@ -1129,7 +1129,7 @@
         <v>39</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C36" s="4">
         <v>75</v>
@@ -1143,7 +1143,7 @@
         <v>40</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" s="4">
         <v>66</v>
@@ -1157,7 +1157,7 @@
         <v>41</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C38" s="4">
         <v>20</v>
@@ -1188,7 +1188,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C41" s="15">
         <f>SUM(C9,C15,C21,C28,C34,C39)</f>
@@ -1211,7 +1211,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B44" s="14" t="s">
         <v>17</v>
@@ -1236,42 +1236,42 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>

</xml_diff>